<commit_message>
Distinguish between aw and ww heat pump in esys generator #308
</commit_message>
<xml_diff>
--- a/pycity_calc/cities/scripts/input_esys_generator/city_clust_simple_enersys.xlsx
+++ b/pycity_calc/cities/scripts/input_esys_generator/city_clust_simple_enersys.xlsx
@@ -369,7 +369,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>